<commit_message>
More organization validation updates
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-eicr-anon-document-bundle.xlsx
+++ b/output/StructureDefinition-eicr-anon-document-bundle.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-18T16:49:21+10:00</t>
+    <t>2024-06-18T18:40:58+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -583,7 +583,7 @@
   </si>
   <si>
     <t>bdl-5:must be a resource unless there's a request or response {resource.exists() or request.exists() or response.exists()}
-bdl-8:fullUrl cannot be a version specific reference {fullUrl.contains('/_history/').not()}ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}eicr-anon-org-tele:All Organization resources (other than PHAs in RR) must conform to EICRAnonymizedOrgTele {resource.ofType(Organization).empty() or resource.ofType(Organization).where(type.coding.code='RR7' or type.coding.code='RR8' or type.coding.code='RR12') or where(resource.ofType(Organization)).fullUrl.resolve().conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-org-tele')}</t>
+bdl-8:fullUrl cannot be a version specific reference {fullUrl.contains('/_history/').not()}ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}eicr-anon-org-tele:All Organization resources (other than PHAs in RR) must conform to EICRAnonymizedOrgTele {resource.ofType(Organization).empty() or resource.ofType(Organization).where(type.coding.code='RR7' or type.coding.code='RR8' or type.coding.code='RR12') or where(resource is Organization).fullUrl.resolve().conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-org-tele')}eicr-anon-org-tele-addr:All Organization resources (other than custodian and PHAs in RR) must conform to EICRAnonymizedOrgTeleAddr {resource.ofType(Organization).empty() or resource.ofType(Organization).where(type.coding.code='RR7' or type.coding.code='RR8' or type.coding.code='RR12') or resource.ofType(Organization).where(%context.fullUrl.endsWith(%rootResource.entry.resource.ofType(Composition).custodian.reference)) or where(resource is Organization).fullUrl.resolve().conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-org-tele-addr')}</t>
   </si>
   <si>
     <t>Bundle.entry.id</t>

</xml_diff>

<commit_message>
Update to Organization processing
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-eicr-anon-document-bundle.xlsx
+++ b/output/StructureDefinition-eicr-anon-document-bundle.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-18T18:40:58+10:00</t>
+    <t>2024-06-21T10:51:28+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -583,7 +583,24 @@
   </si>
   <si>
     <t>bdl-5:must be a resource unless there's a request or response {resource.exists() or request.exists() or response.exists()}
-bdl-8:fullUrl cannot be a version specific reference {fullUrl.contains('/_history/').not()}ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}eicr-anon-org-tele:All Organization resources (other than PHAs in RR) must conform to EICRAnonymizedOrgTele {resource.ofType(Organization).empty() or resource.ofType(Organization).where(type.coding.code='RR7' or type.coding.code='RR8' or type.coding.code='RR12') or where(resource is Organization).fullUrl.resolve().conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-org-tele')}eicr-anon-org-tele-addr:All Organization resources (other than custodian and PHAs in RR) must conform to EICRAnonymizedOrgTeleAddr {resource.ofType(Organization).empty() or resource.ofType(Organization).where(type.coding.code='RR7' or type.coding.code='RR8' or type.coding.code='RR12') or resource.ofType(Organization).where(%context.fullUrl.endsWith(%rootResource.entry.resource.ofType(Composition).custodian.reference)) or where(resource is Organization).fullUrl.resolve().conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-org-tele-addr')}</t>
+bdl-8:fullUrl cannot be a version specific reference {fullUrl.contains('/_history/').not()}ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}eicr-anon-org-tele:All Organization resources (other than in lab orders, lab results, and PHAs in RR) must conform to EICRAnonymizedOrgTele {resource.ofType(Organization).empty() or 
+                resource.ofType(Organization).where(type.coding.code.first()='RR7' or type.coding.code.first()='RR8' or type.coding.code.first()='RR12') or 
+                resource.ofType(Organization).where(
+                                      ('Organization/' + id in %rootResource.entry.resource.ofType(ServiceRequest).descendants().reference).trace('in1') and 
+                                      (
+                                        'Organization/' + id in %rootResource.entry.resource.exclude(%rootResource.entry.resource.ofType(ServiceRequest)).descendants().reference
+                                      ).not().trace('in2')
+                                    ).trace('where') or 
+                where(resource is Organization).fullUrl.resolve().conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-org-tele')}eicr-anon-org-tele-addr:All Organization resources (other than custodian, in laborders, lab results, and PHAs in RR) must conform to EICRAnonymizedOrgTeleAddr {resource.ofType(Organization).empty() or 
+resource.ofType(Organization).where(type.coding.code.first()='RR7' or type.coding.code.first()='RR8' or type.coding.code.first()='RR12') or 
+resource.ofType(Organization).where(%context.fullUrl.endsWith(%rootResource.entry.resource.ofType(Composition).custodian.reference)) or 
+resource.ofType(Organization).where(
+                                      ('Organization/' + id in %rootResource.entry.resource.ofType(ServiceRequest).descendants().reference).trace('in1') and 
+                                      (
+                                        'Organization/' + id in %rootResource.entry.resource.exclude(%rootResource.entry.resource.ofType(ServiceRequest)).descendants().reference
+                                      ).not().trace('in2')
+                                    ).trace('where') or 
+where(resource is Organization).fullUrl.resolve().conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-org-tele-addr')}</t>
   </si>
   <si>
     <t>Bundle.entry.id</t>

</xml_diff>

<commit_message>
Refactor invariants Add text constraints Added practitioner testing file
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-eicr-anon-document-bundle.xlsx
+++ b/output/StructureDefinition-eicr-anon-document-bundle.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2928" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2928" uniqueCount="311">
   <si>
     <t>Property</t>
   </si>
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-26T06:54:29+10:00</t>
+    <t>2024-06-28T19:57:37+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -263,7 +263,7 @@
   </si>
   <si>
     <t>bdl-1:total only when a search or history {total.empty() or (type = 'searchset') or (type = 'history')}
-bdl-2:entry.search only when a search {entry.search.empty() or (type = 'searchset')}bdl-3:entry.request mandatory for batch/transaction/history, otherwise prohibited {entry.all(request.exists() = (%resource.type = 'batch' or %resource.type = 'transaction' or %resource.type = 'history'))}bdl-4:entry.response mandatory for batch-response/transaction-response/history, otherwise prohibited {entry.all(response.exists() = (%resource.type = 'batch-response' or %resource.type = 'transaction-response' or %resource.type = 'history'))}bdl-7:FullUrl must be unique in a bundle, or else entries with the same fullUrl must have different meta.versionId (except in history bundles) {(type = 'history') or entry.where(fullUrl.exists()).select(fullUrl&amp;resource.meta.versionId).isDistinct()}bdl-9:A document must have an identifier with a system and a value {type = 'document' implies (identifier.system.exists() and identifier.value.exists())}bdl-10:A document must have a date {type = 'document' implies (timestamp.hasValue())}bdl-11:A document must have a Composition as the first resource {type = 'document' implies entry.first().resource.is(Composition)}bdl-12:A message must have a MessageHeader as the first resource {type = 'message' implies entry.first().resource.is(MessageHeader)}eicr-anon-patient:All Patient resources must conform to EICRAnonymizedPatient profile {entry.resource.ofType(Patient).empty() or entry.where(resource.ofType(Patient).exists()).fullUrl.resolve().conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-patient')}eicr-anon-prct:All Practitioner resources must conform to EICRAnonymizedPractitioner {entry.resource.ofType(Practitioner).empty() or entry.where(resource.ofType(Practitioner).exists()).fullUrl.resolve().conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-practitioner')}eicr-anon-prct-rol:All PractitionerRole resources must conform to EICRAnonymizedPractitionerRole {entry.resource.ofType(PractitionerRole).empty() or entry.where(resource.ofType(PractitionerRole).exists()).fullUrl.resolve().conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-practitionerrole')}eicr-anon-enc:All Encounter resources must conform to EICRAnonymizedEncounter {entry.resource.ofType(Encounter).empty() or entry.where(resource.ofType(Encounter).exists()).fullUrl.resolve().conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-encounter')}eicr-anon-rp:All RelatedPerson resources must conform to EICRAnonymizedRelatedPerson {entry.resource.ofType(RelatedPerson).empty() or entry.where(resource.ofType(RelatedPerson).exists()).fullUrl.resolve().conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-relatedperson')}eicr-anon-exposure:US Public Health Exposure Contact Information is not allowed {entry.fullUrl.resolve().conformsTo('http://hl7.org/fhir/us/ecr/StructureDefinition/us-ph-exposure-contact-information').not()}</t>
+bdl-2:entry.search only when a search {entry.search.empty() or (type = 'searchset')}bdl-3:entry.request mandatory for batch/transaction/history, otherwise prohibited {entry.all(request.exists() = (%resource.type = 'batch' or %resource.type = 'transaction' or %resource.type = 'history'))}bdl-4:entry.response mandatory for batch-response/transaction-response/history, otherwise prohibited {entry.all(response.exists() = (%resource.type = 'batch-response' or %resource.type = 'transaction-response' or %resource.type = 'history'))}bdl-7:FullUrl must be unique in a bundle, or else entries with the same fullUrl must have different meta.versionId (except in history bundles) {(type = 'history') or entry.where(fullUrl.exists()).select(fullUrl&amp;resource.meta.versionId).isDistinct()}bdl-9:A document must have an identifier with a system and a value {type = 'document' implies (identifier.system.exists() and identifier.value.exists())}bdl-10:A document must have a date {type = 'document' implies (timestamp.hasValue())}bdl-11:A document must have a Composition as the first resource {type = 'document' implies entry.first().resource.is(Composition)}bdl-12:A message must have a MessageHeader as the first resource {type = 'message' implies entry.first().resource.is(MessageHeader)}</t>
   </si>
   <si>
     <t>N/A</t>
@@ -581,7 +581,7 @@
   </si>
   <si>
     <t>bdl-5:must be a resource unless there's a request or response {resource.exists() or request.exists() or response.exists()}
-bdl-8:fullUrl cannot be a version specific reference {fullUrl.contains('/_history/').not()}ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}</t>
+bdl-8:fullUrl cannot be a version specific reference {fullUrl.contains('/_history/').not()}ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}eicr-anon-text-div:text.div SHALL be '&lt;div xmlns="http://www.w3.org/1999/xhtml"&gt;&lt;p&gt;MASKED&lt;/p&gt;&lt;/div&gt;' {resource.text.`div` ~ '&lt;div xmlns="http://www.w3.org/1999/xhtml"&gt;&lt;p&gt;MASKED&lt;/p&gt;&lt;/div&gt;'}eicr-anon-patient:All Patient resources must conform to EICRAnonymizedPatient profile {resource.ofType(Patient).empty() or resource.ofType(Patient).conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-patient')}eicr-anon-prct:All Practitioner resources must conform to EICRAnonymizedPractitioner {resource.ofType(Practitioner).empty() or resource.ofType(Practitioner).conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-practitioner')}eicr-anon-prct-rol:All PractitionerRole resources must conform to EICRAnonymizedPractitionerRole {resource.ofType(PractitionerRole).empty() or resource.ofType(PractitionerRole).conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-practitionerrole')}eicr-anon-enc:All Encounter resources must conform to EICRAnonymizedEncounter {resource.ofType(Encounter).empty() or resource.ofType(Encounter).conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-encounter')}eicr-anon-rp:All RelatedPerson resources must conform to EICRAnonymizedRelatedPerson {resource.ofType(RelatedPerson).empty() or resource.ofType(RelatedPerson).conformsTo('http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-relatedperson')}eicr-anon-exposure:US Public Health Exposure Contact Information is not allowed {resource.conformsTo('http://hl7.org/fhir/us/ecr/StructureDefinition/us-ph-exposure-contact-information').not()}</t>
   </si>
   <si>
     <t>Bundle.entry.id</t>
@@ -854,6 +854,10 @@
   </si>
   <si>
     <t>slicePublicHealthComposition</t>
+  </si>
+  <si>
+    <t>bdl-5:must be a resource unless there's a request or response {resource.exists() or request.exists() or response.exists()}
+bdl-8:fullUrl cannot be a version specific reference {fullUrl.contains('/_history/').not()}ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}</t>
   </si>
   <si>
     <t>Bundle.entry:slicePublicHealthComposition.id</t>
@@ -6903,7 +6907,7 @@
         <v>75</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>178</v>
+        <v>266</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>75</v>
@@ -6920,7 +6924,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B50" t="s" s="2">
         <v>179</v>
@@ -7032,7 +7036,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B51" t="s" s="2">
         <v>180</v>
@@ -7146,7 +7150,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B52" t="s" s="2">
         <v>181</v>
@@ -7262,7 +7266,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B53" t="s" s="2">
         <v>182</v>
@@ -7374,7 +7378,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B54" t="s" s="2">
         <v>185</v>
@@ -7488,7 +7492,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B55" t="s" s="2">
         <v>189</v>
@@ -7514,16 +7518,16 @@
         <v>75</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" t="s" s="2">
@@ -7585,16 +7589,16 @@
         <v>75</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>75</v>
@@ -7602,7 +7606,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B56" t="s" s="2">
         <v>194</v>
@@ -7714,7 +7718,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B57" t="s" s="2">
         <v>198</v>
@@ -7826,7 +7830,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B58" t="s" s="2">
         <v>199</v>
@@ -7940,7 +7944,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B59" t="s" s="2">
         <v>200</v>
@@ -8056,7 +8060,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B60" t="s" s="2">
         <v>201</v>
@@ -8170,7 +8174,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B61" t="s" s="2">
         <v>207</v>
@@ -8284,7 +8288,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B62" t="s" s="2">
         <v>212</v>
@@ -8396,7 +8400,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B63" t="s" s="2">
         <v>216</v>
@@ -8508,7 +8512,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B64" t="s" s="2">
         <v>217</v>
@@ -8622,7 +8626,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B65" t="s" s="2">
         <v>218</v>
@@ -8738,7 +8742,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B66" t="s" s="2">
         <v>219</v>
@@ -8850,7 +8854,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B67" t="s" s="2">
         <v>224</v>
@@ -8964,7 +8968,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B68" t="s" s="2">
         <v>228</v>
@@ -9076,7 +9080,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B69" t="s" s="2">
         <v>231</v>
@@ -9188,7 +9192,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B70" t="s" s="2">
         <v>233</v>
@@ -9300,7 +9304,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B71" t="s" s="2">
         <v>236</v>
@@ -9412,7 +9416,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B72" t="s" s="2">
         <v>239</v>
@@ -9524,7 +9528,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B73" t="s" s="2">
         <v>243</v>
@@ -9636,7 +9640,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B74" t="s" s="2">
         <v>244</v>
@@ -9750,7 +9754,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B75" t="s" s="2">
         <v>245</v>
@@ -9866,7 +9870,7 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B76" t="s" s="2">
         <v>246</v>
@@ -9978,7 +9982,7 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B77" t="s" s="2">
         <v>249</v>
@@ -10090,7 +10094,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B78" t="s" s="2">
         <v>252</v>
@@ -10204,7 +10208,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B79" t="s" s="2">
         <v>256</v>
@@ -10318,7 +10322,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B80" t="s" s="2">
         <v>260</v>
@@ -10432,10 +10436,10 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -10458,19 +10462,19 @@
         <v>86</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="N81" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="O81" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="P81" t="s" s="2">
         <v>75</v>
@@ -10519,7 +10523,7 @@
         <v>75</v>
       </c>
       <c r="AF81" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AG81" t="s" s="2">
         <v>76</v>

</xml_diff>